<commit_message>
TRDK-38: Exponential Moving Average
</commit_message>
<xml_diff>
--- a/sources/Tests/Indicators.xlsx
+++ b/sources/Tests/Indicators.xlsx
@@ -934,7 +934,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G113" sqref="G113"/>
+      <selection pane="bottomLeft" activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -946,7 +946,7 @@
     <col min="5" max="5" width="2.5703125" style="11" customWidth="1"/>
     <col min="6" max="6" width="9.140625" style="14"/>
     <col min="7" max="7" width="2.140625" style="11" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="3" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="3" customWidth="1"/>
     <col min="9" max="9" width="9.140625" style="17"/>
     <col min="10" max="10" width="2.28515625" style="11" customWidth="1"/>
   </cols>
@@ -1448,7 +1448,7 @@
         <v>0.18181818181818182</v>
       </c>
       <c r="I16" s="17">
-        <f t="shared" si="1"/>
+        <f>H16*(C16-I15)+I15</f>
         <v>1115.7739002495539</v>
       </c>
       <c r="J16" s="11" t="s">
@@ -4822,7 +4822,7 @@
       </c>
       <c r="G113" s="14"/>
       <c r="H113" s="14">
-        <f t="shared" ref="G113:I113" si="9">COUNTIF(H2:H112, "&gt;0")</f>
+        <f t="shared" ref="H113:I113" si="9">COUNTIF(H2:H112, "&gt;0")</f>
         <v>111</v>
       </c>
       <c r="I113" s="14">

</xml_diff>

<commit_message>
TRDK-39: Smoothed Moving Average.
</commit_message>
<xml_diff>
--- a/sources/Tests/Indicators.xlsx
+++ b/sources/Tests/Indicators.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1004" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1114" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -666,7 +666,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
@@ -701,21 +701,18 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="166" fontId="18" fillId="39" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="166" fontId="0" fillId="39" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="4" fontId="17" fillId="25" borderId="0" xfId="34" applyNumberFormat="1"/>
-    <xf numFmtId="4" fontId="26" fillId="25" borderId="0" xfId="34" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="4" fontId="8" fillId="4" borderId="0" xfId="8" applyNumberFormat="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="4" fontId="18" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="4" fontId="21" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="4" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="4" fontId="18" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="4" fontId="21" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="4" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="4" fontId="18" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="4" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="4" fontId="17" fillId="25" borderId="0" xfId="34" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="18" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="21" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="8" fillId="4" borderId="0" xfId="8" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="18" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="21" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="26" fillId="25" borderId="0" xfId="34" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="17" fillId="25" borderId="0" xfId="34" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="17" fillId="25" borderId="0" xfId="34" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1038,50 +1035,51 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J113"/>
+  <dimension ref="A1:K113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H113" sqref="H113"/>
+      <selection pane="bottomLeft" activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.7109375" style="33" customWidth="1"/>
     <col min="2" max="2" width="2" style="7" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="45"/>
+    <col min="3" max="3" width="9.140625" style="35"/>
     <col min="4" max="4" width="2.5703125" style="9" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="43"/>
+    <col min="5" max="5" width="9.140625" style="11"/>
     <col min="6" max="6" width="2.140625" style="9" customWidth="1"/>
     <col min="7" max="7" width="9.140625" style="2" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="40"/>
+    <col min="8" max="8" width="9.140625" style="12"/>
     <col min="9" max="9" width="1.7109375" style="9" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="34"/>
+    <col min="10" max="10" width="9.140625" style="43"/>
+    <col min="11" max="11" width="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="18"/>
-      <c r="C1" s="37"/>
+      <c r="C1" s="22"/>
       <c r="D1" s="21"/>
-      <c r="E1" s="37"/>
+      <c r="E1" s="22"/>
       <c r="F1" s="21"/>
-      <c r="H1" s="37"/>
+      <c r="H1" s="22"/>
       <c r="I1" s="21"/>
-      <c r="J1"/>
-    </row>
-    <row r="2" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J1" s="40"/>
+    </row>
+    <row r="2" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="6"/>
-      <c r="C2" s="44" t="s">
+      <c r="C2" s="34" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="8"/>
-      <c r="E2" s="41" t="s">
+      <c r="E2" s="10" t="s">
         <v>2</v>
       </c>
       <c r="F2" s="8"/>
@@ -1092,24 +1090,25 @@
         <v>4</v>
       </c>
       <c r="I2" s="8"/>
-      <c r="J2" s="35" t="s">
+      <c r="J2" s="41" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K2" s="9"/>
+    </row>
+    <row r="3" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="33">
         <v>41435</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="45">
+      <c r="C3" s="35">
         <v>1642.81</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="42">
+      <c r="E3" s="36">
         <v>0</v>
       </c>
       <c r="F3" s="9" t="s">
@@ -1125,24 +1124,27 @@
       <c r="I3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J3" s="46">
+      <c r="J3" s="42">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K3" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="33">
         <v>41436</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="45">
+      <c r="C4" s="35">
         <v>1626.13</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="42">
+      <c r="E4" s="36">
         <v>0</v>
       </c>
       <c r="F4" s="9" t="s">
@@ -1158,24 +1160,27 @@
       <c r="I4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J4" s="46">
+      <c r="J4" s="42">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K4" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="33">
         <v>41437</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="45">
+      <c r="C5" s="35">
         <v>1612.52</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="42">
+      <c r="E5" s="36">
         <v>0</v>
       </c>
       <c r="F5" s="9" t="s">
@@ -1191,24 +1196,27 @@
       <c r="I5" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J5" s="46">
+      <c r="J5" s="42">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K5" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="33">
         <v>41438</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="45">
+      <c r="C6" s="35">
         <v>1636.36</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="42">
+      <c r="E6" s="36">
         <v>0</v>
       </c>
       <c r="F6" s="9" t="s">
@@ -1224,24 +1232,27 @@
       <c r="I6" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J6" s="46">
+      <c r="J6" s="42">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K6" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="33">
         <v>41439</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="45">
+      <c r="C7" s="35">
         <v>1626.73</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="42">
+      <c r="E7" s="36">
         <v>0</v>
       </c>
       <c r="F7" s="9" t="s">
@@ -1257,24 +1268,27 @@
       <c r="I7" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J7" s="46">
+      <c r="J7" s="42">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K7" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="33">
         <v>41442</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="45">
+      <c r="C8" s="35">
         <v>1639.04</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="42">
+      <c r="E8" s="36">
         <v>0</v>
       </c>
       <c r="F8" s="9" t="s">
@@ -1290,24 +1304,27 @@
       <c r="I8" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J8" s="46">
+      <c r="J8" s="42">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K8" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="33">
         <v>41443</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="45">
+      <c r="C9" s="35">
         <v>1651.81</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="42">
+      <c r="E9" s="36">
         <v>0</v>
       </c>
       <c r="F9" s="9" t="s">
@@ -1323,24 +1340,27 @@
       <c r="I9" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J9" s="46">
+      <c r="J9" s="42">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K9" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="33">
         <v>41444</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="45">
+      <c r="C10" s="35">
         <v>1628.93</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="43">
+      <c r="E10" s="11">
         <v>0</v>
       </c>
       <c r="F10" s="9" t="s">
@@ -1356,24 +1376,27 @@
       <c r="I10" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J10" s="46">
+      <c r="J10" s="42">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K10" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="33">
         <v>41445</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="45">
+      <c r="C11" s="35">
         <v>1588.19</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="43">
+      <c r="E11" s="11">
         <v>0</v>
       </c>
       <c r="F11" s="9" t="s">
@@ -1389,24 +1412,27 @@
       <c r="I11" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J11" s="46">
+      <c r="J11" s="42">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K11" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="33">
         <v>41446</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="45">
+      <c r="C12" s="35">
         <v>1592.43</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E12" s="43">
+      <c r="E12" s="11">
         <f t="shared" ref="E12:E27" si="2">AVERAGE(C3:C12)</f>
         <v>1624.4950000000001</v>
       </c>
@@ -1417,32 +1443,35 @@
         <f t="shared" si="1"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H12" s="40">
+      <c r="H12" s="12">
         <f>G12*(C12-E12)+E12</f>
         <v>1618.6650000000002</v>
       </c>
       <c r="I12" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J12" s="34">
+      <c r="J12" s="43">
         <f>E12</f>
         <v>1624.4950000000001</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K12" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="33">
         <v>41449</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="45">
+      <c r="C13" s="35">
         <v>1573.09</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E13" s="43">
+      <c r="E13" s="11">
         <f t="shared" si="2"/>
         <v>1617.5230000000001</v>
       </c>
@@ -1453,32 +1482,35 @@
         <f t="shared" si="1"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H13" s="40">
+      <c r="H13" s="12">
         <f t="shared" ref="H13:H27" si="3">G13*(C13-H12)+H12</f>
         <v>1610.3786363636366</v>
       </c>
       <c r="I13" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J13" s="34">
+      <c r="J13" s="43">
         <f>((J12 * COUNT(C4:C13))-J12+C13)/COUNT(C4:C13)</f>
         <v>1619.3544999999999</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K13" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="33">
         <v>41450</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="45">
+      <c r="C14" s="35">
         <v>1588.03</v>
       </c>
       <c r="D14" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E14" s="43">
+      <c r="E14" s="11">
         <f t="shared" si="2"/>
         <v>1613.7130000000002</v>
       </c>
@@ -1489,32 +1521,35 @@
         <f t="shared" si="1"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H14" s="40">
+      <c r="H14" s="12">
         <f t="shared" si="3"/>
         <v>1606.3152479338844</v>
       </c>
       <c r="I14" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J14" s="34">
+      <c r="J14" s="43">
         <f>((J13 * COUNT(C5:C14))-J13+C14)/COUNT(C5:C14)</f>
         <v>1616.2220499999999</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K14" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="33">
         <v>41451</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="45">
+      <c r="C15" s="35">
         <v>1603.26</v>
       </c>
       <c r="D15" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E15" s="43">
+      <c r="E15" s="11">
         <f t="shared" si="2"/>
         <v>1612.7870000000003</v>
       </c>
@@ -1525,32 +1560,35 @@
         <f t="shared" si="1"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H15" s="40">
+      <c r="H15" s="12">
         <f t="shared" si="3"/>
         <v>1605.7597483095417</v>
       </c>
       <c r="I15" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J15" s="34">
+      <c r="J15" s="43">
         <f>((J14 * COUNT(C6:C15))-J14+C15)/COUNT(C6:C15)</f>
         <v>1614.925845</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K15" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="33">
         <v>41452</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="45">
+      <c r="C16" s="35">
         <v>1613.2</v>
       </c>
       <c r="D16" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E16" s="43">
+      <c r="E16" s="11">
         <f t="shared" si="2"/>
         <v>1610.4710000000002</v>
       </c>
@@ -1561,32 +1599,35 @@
         <f t="shared" si="1"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H16" s="40">
+      <c r="H16" s="12">
         <f t="shared" si="3"/>
         <v>1607.1125213441705</v>
       </c>
       <c r="I16" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J16" s="34">
+      <c r="J16" s="43">
         <f>((J15 * COUNT(C7:C16))-J15+C16)/COUNT(C7:C16)</f>
         <v>1614.7532605000001</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K16" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="33">
         <v>41453</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="45">
+      <c r="C17" s="35">
         <v>1606.28</v>
       </c>
       <c r="D17" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E17" s="43">
+      <c r="E17" s="11">
         <f t="shared" si="2"/>
         <v>1608.4260000000002</v>
       </c>
@@ -1597,32 +1638,35 @@
         <f t="shared" si="1"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H17" s="40">
+      <c r="H17" s="12">
         <f t="shared" si="3"/>
         <v>1606.9611538270485</v>
       </c>
       <c r="I17" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J17" s="34">
+      <c r="J17" s="43">
         <f>((J16 * COUNT(C8:C17))-J16+C17)/COUNT(C8:C17)</f>
         <v>1613.9059344500001</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K17" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="33">
         <v>41456</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="45">
+      <c r="C18" s="35">
         <v>1614.96</v>
       </c>
       <c r="D18" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E18" s="43">
+      <c r="E18" s="11">
         <f t="shared" si="2"/>
         <v>1606.0180000000005</v>
       </c>
@@ -1633,32 +1677,35 @@
         <f t="shared" si="1"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H18" s="40">
+      <c r="H18" s="12">
         <f t="shared" si="3"/>
         <v>1608.4154894948579</v>
       </c>
       <c r="I18" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J18" s="34">
+      <c r="J18" s="43">
         <f>((J17 * COUNT(C9:C18))-J17+C18)/COUNT(C9:C18)</f>
         <v>1614.0113410050003</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K18" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="33">
         <v>41457</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="45">
+      <c r="C19" s="35">
         <v>1614.08</v>
       </c>
       <c r="D19" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E19" s="43">
+      <c r="E19" s="11">
         <f t="shared" si="2"/>
         <v>1602.2450000000003</v>
       </c>
@@ -1669,32 +1716,35 @@
         <f t="shared" si="1"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H19" s="40">
+      <c r="H19" s="12">
         <f t="shared" si="3"/>
         <v>1609.4454004957927</v>
       </c>
       <c r="I19" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J19" s="34">
+      <c r="J19" s="43">
         <f>((J18 * COUNT(C10:C19))-J18+C19)/COUNT(C10:C19)</f>
         <v>1614.0182069045002</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K19" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="33">
         <v>41458</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="45">
+      <c r="C20" s="35">
         <v>1615.41</v>
       </c>
       <c r="D20" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E20" s="43">
+      <c r="E20" s="11">
         <f t="shared" si="2"/>
         <v>1600.8930000000003</v>
       </c>
@@ -1705,32 +1755,35 @@
         <f t="shared" si="1"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H20" s="40">
+      <c r="H20" s="12">
         <f t="shared" si="3"/>
         <v>1610.5298731329212</v>
       </c>
       <c r="I20" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J20" s="34">
+      <c r="J20" s="43">
         <f>((J19 * COUNT(C11:C20))-J19+C20)/COUNT(C11:C20)</f>
         <v>1614.1573862140501</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K20" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="33">
         <v>41460</v>
       </c>
       <c r="B21" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="45">
+      <c r="C21" s="35">
         <v>1631.89</v>
       </c>
       <c r="D21" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E21" s="43">
+      <c r="E21" s="11">
         <f t="shared" si="2"/>
         <v>1605.2629999999999</v>
       </c>
@@ -1741,32 +1794,35 @@
         <f t="shared" si="1"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H21" s="40">
+      <c r="H21" s="12">
         <f t="shared" si="3"/>
         <v>1614.4135325632992</v>
       </c>
       <c r="I21" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J21" s="34">
+      <c r="J21" s="43">
         <f>((J20 * COUNT(C12:C21))-J20+C21)/COUNT(C12:C21)</f>
         <v>1615.9306475926451</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K21" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="33">
         <v>41463</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C22" s="45">
+      <c r="C22" s="35">
         <v>1640.46</v>
       </c>
       <c r="D22" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E22" s="43">
+      <c r="E22" s="11">
         <f t="shared" si="2"/>
         <v>1610.066</v>
       </c>
@@ -1777,32 +1833,35 @@
         <f t="shared" si="1"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H22" s="40">
+      <c r="H22" s="12">
         <f t="shared" si="3"/>
         <v>1619.1492539154267</v>
       </c>
       <c r="I22" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J22" s="34">
+      <c r="J22" s="43">
         <f>((J21 * COUNT(C13:C22))-J21+C22)/COUNT(C13:C22)</f>
         <v>1618.3835828333806</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K22" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="33">
         <v>41464</v>
       </c>
       <c r="B23" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C23" s="45">
+      <c r="C23" s="35">
         <v>1652.32</v>
       </c>
       <c r="D23" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E23" s="43">
+      <c r="E23" s="11">
         <f t="shared" si="2"/>
         <v>1617.989</v>
       </c>
@@ -1813,32 +1872,35 @@
         <f t="shared" si="1"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H23" s="40">
+      <c r="H23" s="12">
         <f t="shared" si="3"/>
         <v>1625.1802986580765</v>
       </c>
       <c r="I23" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J23" s="34">
+      <c r="J23" s="43">
         <f>((J22 * COUNT(C14:C23))-J22+C23)/COUNT(C14:C23)</f>
         <v>1621.7772245500423</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K23" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="33">
         <v>41465</v>
       </c>
       <c r="B24" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C24" s="45">
+      <c r="C24" s="35">
         <v>1652.62</v>
       </c>
       <c r="D24" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E24" s="43">
+      <c r="E24" s="11">
         <f t="shared" si="2"/>
         <v>1624.4479999999999</v>
       </c>
@@ -1849,32 +1911,35 @@
         <f t="shared" si="1"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H24" s="40">
+      <c r="H24" s="12">
         <f t="shared" si="3"/>
         <v>1630.1693352656989</v>
       </c>
       <c r="I24" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J24" s="34">
+      <c r="J24" s="43">
         <f>((J23 * COUNT(C15:C24))-J23+C24)/COUNT(C15:C24)</f>
         <v>1624.8615020950378</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K24" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="33">
         <v>41466</v>
       </c>
       <c r="B25" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C25" s="45">
+      <c r="C25" s="35">
         <v>1675.02</v>
       </c>
       <c r="D25" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E25" s="43">
+      <c r="E25" s="11">
         <f t="shared" si="2"/>
         <v>1631.6239999999998</v>
       </c>
@@ -1885,32 +1950,35 @@
         <f t="shared" si="1"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H25" s="40">
+      <c r="H25" s="12">
         <f t="shared" si="3"/>
         <v>1638.3240015810263</v>
       </c>
       <c r="I25" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J25" s="34">
+      <c r="J25" s="43">
         <f>((J24 * COUNT(C16:C25))-J24+C25)/COUNT(C16:C25)</f>
         <v>1629.8773518855342</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K25" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="33">
         <v>41467</v>
       </c>
       <c r="B26" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C26" s="45">
+      <c r="C26" s="35">
         <v>1680.19</v>
       </c>
       <c r="D26" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E26" s="43">
+      <c r="E26" s="11">
         <f t="shared" si="2"/>
         <v>1638.3230000000001</v>
       </c>
@@ -1921,32 +1989,35 @@
         <f t="shared" si="1"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H26" s="40">
+      <c r="H26" s="12">
         <f t="shared" si="3"/>
         <v>1645.936001293567</v>
       </c>
       <c r="I26" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J26" s="34">
+      <c r="J26" s="43">
         <f>((J25 * COUNT(C17:C26))-J25+C26)/COUNT(C17:C26)</f>
         <v>1634.9086166969807</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K26" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="33">
         <v>41470</v>
       </c>
       <c r="B27" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C27" s="45">
+      <c r="C27" s="35">
         <v>1682.5</v>
       </c>
       <c r="D27" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E27" s="43">
+      <c r="E27" s="11">
         <f t="shared" si="2"/>
         <v>1645.9450000000004</v>
       </c>
@@ -1957,29 +2028,32 @@
         <f t="shared" si="1"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H27" s="40">
+      <c r="H27" s="12">
         <f t="shared" si="3"/>
         <v>1652.5840010583729</v>
       </c>
       <c r="I27" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J27" s="34">
+      <c r="J27" s="43">
         <f>((J26 * COUNT(C18:C27))-J26+C27)/COUNT(C18:C27)</f>
         <v>1639.6677550272827</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K27" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B28" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C28" s="45">
+      <c r="C28" s="35">
         <v>0</v>
       </c>
       <c r="D28" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E28" s="43">
+      <c r="E28" s="11">
         <v>0</v>
       </c>
       <c r="F28" s="9" t="s">
@@ -1988,30 +2062,33 @@
       <c r="G28" s="2">
         <v>0</v>
       </c>
-      <c r="H28" s="40">
+      <c r="H28" s="12">
         <v>0</v>
       </c>
       <c r="I28" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J28" s="34">
+      <c r="J28" s="43">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K28" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="33">
         <v>41471</v>
       </c>
       <c r="B29" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C29" s="45">
+      <c r="C29" s="35">
         <v>1676.26</v>
       </c>
       <c r="D29" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E29" s="36">
+      <c r="E29" s="37">
         <f>AVERAGE(C19:C$27,C$29:C29)</f>
         <v>1652.075</v>
       </c>
@@ -2022,32 +2099,35 @@
         <f t="shared" si="1"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H29" s="36">
+      <c r="H29" s="37">
         <f>G29*(C29-H27)+H27</f>
         <v>1656.8887281386687</v>
       </c>
       <c r="I29" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J29" s="34">
+      <c r="J29" s="37">
         <f>((J27 * COUNT(C19:C$27,C$29:C29))-J27+C29)/COUNT(C19:C$27,C$29:C29)</f>
         <v>1643.3269795245542</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K29" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="33">
         <v>41472</v>
       </c>
       <c r="B30" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C30" s="45">
+      <c r="C30" s="35">
         <v>1680.91</v>
       </c>
       <c r="D30" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E30" s="36">
+      <c r="E30" s="37">
         <f>AVERAGE(C20:C$27,C$29:C30)</f>
         <v>1658.7580000000003</v>
       </c>
@@ -2058,32 +2138,35 @@
         <f t="shared" si="1"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H30" s="40">
+      <c r="H30" s="12">
         <f t="shared" ref="H30:H61" si="4">G30*(C30-H29)+H29</f>
         <v>1661.2562321134562</v>
       </c>
       <c r="I30" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J30" s="34">
+      <c r="J30" s="37">
         <f>((J29 * COUNT(C20:C$27,C$29:C30))-J29+C30)/COUNT(C20:C$27,C$29:C30)</f>
         <v>1647.0852815720987</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K30" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="33">
         <v>41473</v>
       </c>
       <c r="B31" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C31" s="45">
+      <c r="C31" s="35">
         <v>1689.37</v>
       </c>
       <c r="D31" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E31" s="36">
+      <c r="E31" s="37">
         <f>AVERAGE(C21:C$27,C$29:C31)</f>
         <v>1666.154</v>
       </c>
@@ -2094,32 +2177,35 @@
         <f t="shared" si="1"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H31" s="40">
+      <c r="H31" s="12">
         <f t="shared" si="4"/>
         <v>1666.3678262746459</v>
       </c>
       <c r="I31" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J31" s="34">
+      <c r="J31" s="37">
         <f>((J30 * COUNT(C21:C$27,C$29:C31))-J30+C31)/COUNT(C21:C$27,C$29:C31)</f>
         <v>1651.3137534148889</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K31" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="33">
         <v>41474</v>
       </c>
       <c r="B32" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C32" s="45">
+      <c r="C32" s="35">
         <v>1692.09</v>
       </c>
       <c r="D32" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E32" s="36">
+      <c r="E32" s="37">
         <f>AVERAGE(C22:C$27,C$29:C32)</f>
         <v>1672.1740000000002</v>
       </c>
@@ -2130,32 +2216,35 @@
         <f t="shared" si="1"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H32" s="40">
+      <c r="H32" s="12">
         <f t="shared" si="4"/>
         <v>1671.0445851338013</v>
       </c>
       <c r="I32" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J32" s="34">
+      <c r="J32" s="37">
         <f>((J31 * COUNT(C22:C$27,C$29:C32))-J31+C32)/COUNT(C22:C$27,C$29:C32)</f>
         <v>1655.3913780734001</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K32" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="33">
         <v>41477</v>
       </c>
       <c r="B33" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C33" s="45">
+      <c r="C33" s="35">
         <v>1695.53</v>
       </c>
       <c r="D33" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E33" s="36">
+      <c r="E33" s="37">
         <f>AVERAGE(C23:C$27,C$29:C33)</f>
         <v>1677.6809999999998</v>
       </c>
@@ -2166,32 +2255,35 @@
         <f t="shared" si="1"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H33" s="40">
+      <c r="H33" s="12">
         <f t="shared" si="4"/>
         <v>1675.4964787458375</v>
       </c>
       <c r="I33" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J33" s="34">
+      <c r="J33" s="37">
         <f>((J32 * COUNT(C23:C$27,C$29:C33))-J32+C33)/COUNT(C23:C$27,C$29:C33)</f>
         <v>1659.40524026606</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K33" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="33">
         <v>41478</v>
       </c>
       <c r="B34" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C34" s="45">
+      <c r="C34" s="35">
         <v>1692.39</v>
       </c>
       <c r="D34" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E34" s="36">
+      <c r="E34" s="37">
         <f>AVERAGE(C24:C$27,C$29:C34)</f>
         <v>1681.6880000000001</v>
       </c>
@@ -2202,32 +2294,35 @@
         <f t="shared" si="1"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H34" s="40">
+      <c r="H34" s="12">
         <f t="shared" si="4"/>
         <v>1678.5680280647762</v>
       </c>
       <c r="I34" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J34" s="34">
+      <c r="J34" s="37">
         <f>((J33 * COUNT(C24:C$27,C$29:C34))-J33+C34)/COUNT(C24:C$27,C$29:C34)</f>
         <v>1662.703716239454</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K34" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="33">
         <v>41479</v>
       </c>
       <c r="B35" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C35" s="45">
+      <c r="C35" s="35">
         <v>1685.94</v>
       </c>
       <c r="D35" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E35" s="36">
+      <c r="E35" s="37">
         <f>AVERAGE(C25:C$27,C$29:C35)</f>
         <v>1685.02</v>
       </c>
@@ -2238,32 +2333,35 @@
         <f t="shared" si="1"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H35" s="40">
+      <c r="H35" s="12">
         <f t="shared" si="4"/>
         <v>1679.9083865984533</v>
       </c>
       <c r="I35" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J35" s="34">
+      <c r="J35" s="37">
         <f>((J34 * COUNT(C25:C$27,C$29:C35))-J34+C35)/COUNT(C25:C$27,C$29:C35)</f>
         <v>1665.0273446155086</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K35" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="33">
         <v>41480</v>
       </c>
       <c r="B36" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C36" s="45">
+      <c r="C36" s="35">
         <v>1690.25</v>
       </c>
       <c r="D36" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E36" s="36">
+      <c r="E36" s="37">
         <f>AVERAGE(C26:C$27,C$29:C36)</f>
         <v>1686.5430000000001</v>
       </c>
@@ -2274,32 +2372,35 @@
         <f t="shared" si="1"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H36" s="40">
+      <c r="H36" s="12">
         <f t="shared" si="4"/>
         <v>1681.788679944189</v>
       </c>
       <c r="I36" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J36" s="34">
+      <c r="J36" s="37">
         <f>((J35 * COUNT(C26:C$27,C$29:C36))-J35+C36)/COUNT(C26:C$27,C$29:C36)</f>
         <v>1667.5496101539579</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K36" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="33">
         <v>41481</v>
       </c>
       <c r="B37" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C37" s="45">
+      <c r="C37" s="35">
         <v>1691.65</v>
       </c>
       <c r="D37" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E37" s="36">
+      <c r="E37" s="37">
         <f>AVERAGE(C27:C$27,C$29:C37)</f>
         <v>1687.6889999999999</v>
       </c>
@@ -2310,32 +2411,35 @@
         <f t="shared" si="1"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H37" s="40">
+      <c r="H37" s="12">
         <f t="shared" si="4"/>
         <v>1683.5816472270637</v>
       </c>
       <c r="I37" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J37" s="34">
+      <c r="J37" s="37">
         <f>((J36 * COUNT(C27:C$27,C$29:C37))-J36+C37)/COUNT(C27:C$27,C$29:C37)</f>
         <v>1669.9596491385623</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K37" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="33">
         <v>41484</v>
       </c>
       <c r="B38" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C38" s="45">
+      <c r="C38" s="35">
         <v>1685.33</v>
       </c>
       <c r="D38" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E38" s="43">
+      <c r="E38" s="11">
         <f t="shared" ref="E38:E76" si="5">AVERAGE(C29:C38)</f>
         <v>1687.9720000000002</v>
       </c>
@@ -2346,32 +2450,35 @@
         <f t="shared" si="1"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H38" s="40">
+      <c r="H38" s="12">
         <f t="shared" si="4"/>
         <v>1683.8995295494158</v>
       </c>
       <c r="I38" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J38" s="34">
+      <c r="J38" s="43">
         <f>((J37 * COUNT(C29:C38))-J37+C38)/COUNT(C29:C38)</f>
         <v>1671.4966842247061</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K38" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="33">
         <v>41485</v>
       </c>
       <c r="B39" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C39" s="45">
+      <c r="C39" s="35">
         <v>1685.96</v>
       </c>
       <c r="D39" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E39" s="43">
+      <c r="E39" s="11">
         <f t="shared" si="5"/>
         <v>1688.9419999999998</v>
       </c>
@@ -2382,32 +2489,35 @@
         <f t="shared" si="1"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H39" s="40">
+      <c r="H39" s="12">
         <f t="shared" si="4"/>
         <v>1684.274160540431</v>
       </c>
       <c r="I39" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J39" s="34">
+      <c r="J39" s="43">
         <f>((J38 * COUNT(C30:C39))-J38+C39)/COUNT(C30:C39)</f>
         <v>1672.9430158022355</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K39" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="33">
         <v>41486</v>
       </c>
       <c r="B40" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C40" s="45">
+      <c r="C40" s="35">
         <v>1685.73</v>
       </c>
       <c r="D40" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E40" s="43">
+      <c r="E40" s="11">
         <f t="shared" si="5"/>
         <v>1689.4239999999998</v>
       </c>
@@ -2418,32 +2528,35 @@
         <f t="shared" si="1"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H40" s="40">
+      <c r="H40" s="12">
         <f t="shared" si="4"/>
         <v>1684.538858623989</v>
       </c>
       <c r="I40" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J40" s="34">
+      <c r="J40" s="43">
         <f>((J39 * COUNT(C31:C40))-J39+C40)/COUNT(C31:C40)</f>
         <v>1674.221714222012</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K40" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="33">
         <v>41487</v>
       </c>
       <c r="B41" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C41" s="45">
+      <c r="C41" s="35">
         <v>1706.87</v>
       </c>
       <c r="D41" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E41" s="43">
+      <c r="E41" s="11">
         <f t="shared" si="5"/>
         <v>1691.1739999999998</v>
       </c>
@@ -2454,32 +2567,35 @@
         <f t="shared" si="1"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H41" s="40">
+      <c r="H41" s="12">
         <f t="shared" si="4"/>
         <v>1688.5990661469</v>
       </c>
       <c r="I41" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J41" s="34">
+      <c r="J41" s="43">
         <f>((J40 * COUNT(C32:C41))-J40+C41)/COUNT(C32:C41)</f>
         <v>1677.4865427998109</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K41" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="33">
         <v>41488</v>
       </c>
       <c r="B42" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C42" s="45">
+      <c r="C42" s="35">
         <v>1709.67</v>
       </c>
       <c r="D42" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E42" s="43">
+      <c r="E42" s="11">
         <f t="shared" si="5"/>
         <v>1692.932</v>
       </c>
@@ -2490,32 +2606,35 @@
         <f t="shared" si="1"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H42" s="40">
+      <c r="H42" s="12">
         <f t="shared" si="4"/>
         <v>1692.4301450292819</v>
       </c>
       <c r="I42" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J42" s="34">
+      <c r="J42" s="43">
         <f>((J41 * COUNT(C33:C42))-J41+C42)/COUNT(C33:C42)</f>
         <v>1680.7048885198299</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K42" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="33">
         <v>41491</v>
       </c>
       <c r="B43" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C43" s="45">
+      <c r="C43" s="35">
         <v>1707.14</v>
       </c>
       <c r="D43" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E43" s="43">
+      <c r="E43" s="11">
         <f t="shared" si="5"/>
         <v>1694.0930000000001</v>
       </c>
@@ -2526,32 +2645,35 @@
         <f t="shared" si="1"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H43" s="40">
+      <c r="H43" s="12">
         <f t="shared" si="4"/>
         <v>1695.1046641148671</v>
       </c>
       <c r="I43" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J43" s="34">
+      <c r="J43" s="43">
         <f>((J42 * COUNT(C34:C43))-J42+C43)/COUNT(C34:C43)</f>
         <v>1683.3483996678472</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K43" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="33">
         <v>41492</v>
       </c>
       <c r="B44" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C44" s="45">
+      <c r="C44" s="35">
         <v>1697.37</v>
       </c>
       <c r="D44" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E44" s="43">
+      <c r="E44" s="11">
         <f t="shared" si="5"/>
         <v>1694.5909999999999</v>
       </c>
@@ -2562,32 +2684,35 @@
         <f t="shared" si="1"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H44" s="40">
+      <c r="H44" s="12">
         <f t="shared" si="4"/>
         <v>1695.5165433667094</v>
       </c>
       <c r="I44" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J44" s="34">
+      <c r="J44" s="43">
         <f>((J43 * COUNT(C35:C44))-J43+C44)/COUNT(C35:C44)</f>
         <v>1684.7505597010622</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K44" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="33">
         <v>41493</v>
       </c>
       <c r="B45" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C45" s="45">
+      <c r="C45" s="35">
         <v>1690.91</v>
       </c>
       <c r="D45" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E45" s="43">
+      <c r="E45" s="11">
         <f t="shared" si="5"/>
         <v>1695.0880000000002</v>
       </c>
@@ -2598,32 +2723,35 @@
         <f t="shared" si="1"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H45" s="40">
+      <c r="H45" s="12">
         <f t="shared" si="4"/>
         <v>1694.6789900273077</v>
       </c>
       <c r="I45" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J45" s="34">
+      <c r="J45" s="43">
         <f>((J44 * COUNT(C36:C45))-J44+C45)/COUNT(C36:C45)</f>
         <v>1685.3665037309561</v>
       </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K45" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="33">
         <v>41494</v>
       </c>
       <c r="B46" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C46" s="45">
+      <c r="C46" s="35">
         <v>1697.48</v>
       </c>
       <c r="D46" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E46" s="43">
+      <c r="E46" s="11">
         <f t="shared" si="5"/>
         <v>1695.8110000000001</v>
       </c>
@@ -2634,32 +2762,35 @@
         <f t="shared" si="1"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H46" s="40">
+      <c r="H46" s="12">
         <f t="shared" si="4"/>
         <v>1695.1882645677972</v>
       </c>
       <c r="I46" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J46" s="34">
+      <c r="J46" s="43">
         <f>((J45 * COUNT(C37:C46))-J45+C46)/COUNT(C37:C46)</f>
         <v>1686.5778533578607</v>
       </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K46" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="33">
         <v>41495</v>
       </c>
       <c r="B47" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C47" s="45">
+      <c r="C47" s="35">
         <v>1691.42</v>
       </c>
       <c r="D47" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E47" s="43">
+      <c r="E47" s="11">
         <f t="shared" si="5"/>
         <v>1695.7879999999998</v>
       </c>
@@ -2670,32 +2801,35 @@
         <f t="shared" si="1"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H47" s="40">
+      <c r="H47" s="12">
         <f t="shared" si="4"/>
         <v>1694.5031255554704</v>
       </c>
       <c r="I47" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J47" s="34">
+      <c r="J47" s="43">
         <f>((J46 * COUNT(C38:C47))-J46+C47)/COUNT(C38:C47)</f>
         <v>1687.0620680220745</v>
       </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K47" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="33">
         <v>41498</v>
       </c>
       <c r="B48" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C48" s="45">
+      <c r="C48" s="35">
         <v>1689.47</v>
       </c>
       <c r="D48" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E48" s="43">
+      <c r="E48" s="11">
         <f t="shared" si="5"/>
         <v>1696.2019999999998</v>
       </c>
@@ -2706,32 +2840,35 @@
         <f t="shared" si="1"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H48" s="40">
+      <c r="H48" s="12">
         <f t="shared" si="4"/>
         <v>1693.5880118181121</v>
       </c>
       <c r="I48" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J48" s="34">
+      <c r="J48" s="43">
         <f>((J47 * COUNT(C39:C48))-J47+C48)/COUNT(C39:C48)</f>
         <v>1687.3028612198673</v>
       </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K48" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="33">
         <v>41499</v>
       </c>
       <c r="B49" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C49" s="45">
+      <c r="C49" s="35">
         <v>1694.16</v>
       </c>
       <c r="D49" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E49" s="43">
+      <c r="E49" s="11">
         <f t="shared" si="5"/>
         <v>1697.0220000000002</v>
       </c>
@@ -2742,32 +2879,35 @@
         <f t="shared" si="1"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H49" s="40">
+      <c r="H49" s="12">
         <f t="shared" si="4"/>
         <v>1693.6920096693646</v>
       </c>
       <c r="I49" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J49" s="34">
+      <c r="J49" s="43">
         <f>((J48 * COUNT(C40:C49))-J48+C49)/COUNT(C40:C49)</f>
         <v>1687.9885750978806</v>
       </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K49" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="33">
         <v>41500</v>
       </c>
       <c r="B50" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C50" s="45">
+      <c r="C50" s="35">
         <v>1685.39</v>
       </c>
       <c r="D50" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E50" s="43">
+      <c r="E50" s="11">
         <f t="shared" si="5"/>
         <v>1696.9880000000001</v>
       </c>
@@ -2778,32 +2918,35 @@
         <f t="shared" si="1"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H50" s="40">
+      <c r="H50" s="12">
         <f t="shared" si="4"/>
         <v>1692.1825533658437</v>
       </c>
       <c r="I50" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J50" s="34">
+      <c r="J50" s="43">
         <f>((J49 * COUNT(C41:C50))-J49+C50)/COUNT(C41:C50)</f>
         <v>1687.7287175880926</v>
       </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K50" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="33">
         <v>41501</v>
       </c>
       <c r="B51" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C51" s="45">
+      <c r="C51" s="35">
         <v>1661.32</v>
       </c>
       <c r="D51" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E51" s="43">
+      <c r="E51" s="11">
         <f t="shared" si="5"/>
         <v>1692.4329999999998</v>
       </c>
@@ -2814,32 +2957,35 @@
         <f t="shared" si="1"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H51" s="40">
+      <c r="H51" s="12">
         <f t="shared" si="4"/>
         <v>1686.5711800265994</v>
       </c>
       <c r="I51" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J51" s="34">
+      <c r="J51" s="43">
         <f>((J50 * COUNT(C42:C51))-J50+C51)/COUNT(C42:C51)</f>
         <v>1685.0878458292834</v>
       </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K51" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="33">
         <v>41502</v>
       </c>
       <c r="B52" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C52" s="45">
+      <c r="C52" s="35">
         <v>1655.83</v>
       </c>
       <c r="D52" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E52" s="43">
+      <c r="E52" s="11">
         <f t="shared" si="5"/>
         <v>1687.0489999999998</v>
       </c>
@@ -2850,32 +2996,35 @@
         <f t="shared" si="1"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H52" s="40">
+      <c r="H52" s="12">
         <f t="shared" si="4"/>
         <v>1680.9818745672178</v>
       </c>
       <c r="I52" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J52" s="34">
+      <c r="J52" s="43">
         <f>((J51 * COUNT(C43:C52))-J51+C52)/COUNT(C43:C52)</f>
         <v>1682.1620612463551</v>
       </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K52" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="33">
         <v>41505</v>
       </c>
       <c r="B53" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C53" s="45">
+      <c r="C53" s="35">
         <v>1646.06</v>
       </c>
       <c r="D53" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E53" s="43">
+      <c r="E53" s="11">
         <f t="shared" si="5"/>
         <v>1680.941</v>
       </c>
@@ -2886,32 +3035,35 @@
         <f t="shared" si="1"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H53" s="40">
+      <c r="H53" s="12">
         <f t="shared" si="4"/>
         <v>1674.6324428277237</v>
       </c>
       <c r="I53" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J53" s="34">
+      <c r="J53" s="43">
         <f>((J52 * COUNT(C44:C53))-J52+C53)/COUNT(C44:C53)</f>
         <v>1678.5518551217197</v>
       </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K53" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="33">
         <v>41506</v>
       </c>
       <c r="B54" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C54" s="45">
+      <c r="C54" s="35">
         <v>1652.35</v>
       </c>
       <c r="D54" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E54" s="43">
+      <c r="E54" s="11">
         <f t="shared" si="5"/>
         <v>1676.4389999999999</v>
       </c>
@@ -2922,32 +3074,35 @@
         <f t="shared" si="1"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H54" s="40">
+      <c r="H54" s="12">
         <f t="shared" si="4"/>
         <v>1670.5810895863194</v>
       </c>
       <c r="I54" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J54" s="34">
+      <c r="J54" s="43">
         <f>((J53 * COUNT(C45:C54))-J53+C54)/COUNT(C45:C54)</f>
         <v>1675.9316696095477</v>
       </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K54" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="33">
         <v>41507</v>
       </c>
       <c r="B55" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C55" s="45">
+      <c r="C55" s="35">
         <v>1642.8</v>
       </c>
       <c r="D55" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E55" s="43">
+      <c r="E55" s="11">
         <f t="shared" si="5"/>
         <v>1671.6279999999999</v>
       </c>
@@ -2958,32 +3113,35 @@
         <f t="shared" si="1"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H55" s="40">
+      <c r="H55" s="12">
         <f t="shared" si="4"/>
         <v>1665.5299823888067</v>
       </c>
       <c r="I55" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J55" s="34">
+      <c r="J55" s="43">
         <f>((J54 * COUNT(C46:C55))-J54+C55)/COUNT(C46:C55)</f>
         <v>1672.6185026485928</v>
       </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K55" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="33">
         <v>41508</v>
       </c>
       <c r="B56" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C56" s="45">
+      <c r="C56" s="35">
         <v>1656.96</v>
       </c>
       <c r="D56" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E56" s="43">
+      <c r="E56" s="11">
         <f t="shared" si="5"/>
         <v>1667.5759999999998</v>
       </c>
@@ -2994,32 +3152,35 @@
         <f t="shared" si="1"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H56" s="40">
+      <c r="H56" s="12">
         <f t="shared" si="4"/>
         <v>1663.97180377266</v>
       </c>
       <c r="I56" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J56" s="34">
+      <c r="J56" s="43">
         <f>((J55 * COUNT(C47:C56))-J55+C56)/COUNT(C47:C56)</f>
         <v>1671.0526523837336</v>
       </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K56" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="33">
         <v>41509</v>
       </c>
       <c r="B57" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C57" s="45">
+      <c r="C57" s="35">
         <v>1663.5</v>
       </c>
       <c r="D57" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E57" s="43">
+      <c r="E57" s="11">
         <f t="shared" si="5"/>
         <v>1664.7840000000001</v>
       </c>
@@ -3030,32 +3191,35 @@
         <f t="shared" si="1"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H57" s="40">
+      <c r="H57" s="12">
         <f t="shared" si="4"/>
         <v>1663.8860212685399</v>
       </c>
       <c r="I57" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J57" s="34">
+      <c r="J57" s="43">
         <f>((J56 * COUNT(C48:C57))-J56+C57)/COUNT(C48:C57)</f>
         <v>1670.2973871453601</v>
       </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K57" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="33">
         <v>41512</v>
       </c>
       <c r="B58" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C58" s="45">
+      <c r="C58" s="35">
         <v>1656.78</v>
       </c>
       <c r="D58" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E58" s="43">
+      <c r="E58" s="11">
         <f t="shared" si="5"/>
         <v>1661.5149999999999</v>
       </c>
@@ -3066,32 +3230,35 @@
         <f t="shared" si="1"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H58" s="40">
+      <c r="H58" s="12">
         <f t="shared" si="4"/>
         <v>1662.5940174015327</v>
       </c>
       <c r="I58" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J58" s="34">
+      <c r="J58" s="43">
         <f>((J57 * COUNT(C49:C58))-J57+C58)/COUNT(C49:C58)</f>
         <v>1668.9456484308241</v>
       </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K58" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="33">
         <v>41513</v>
       </c>
       <c r="B59" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C59" s="45">
+      <c r="C59" s="35">
         <v>1630.48</v>
       </c>
       <c r="D59" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E59" s="43">
+      <c r="E59" s="11">
         <f t="shared" si="5"/>
         <v>1655.1470000000002</v>
       </c>
@@ -3102,32 +3269,35 @@
         <f t="shared" si="1"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H59" s="40">
+      <c r="H59" s="12">
         <f t="shared" si="4"/>
         <v>1656.7551051467085</v>
       </c>
       <c r="I59" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J59" s="34">
+      <c r="J59" s="43">
         <f>((J58 * COUNT(C50:C59))-J58+C59)/COUNT(C50:C59)</f>
         <v>1665.0990835877415</v>
       </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K59" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="33">
         <v>41514</v>
       </c>
       <c r="B60" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C60" s="45">
+      <c r="C60" s="35">
         <v>1634.96</v>
       </c>
       <c r="D60" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E60" s="43">
+      <c r="E60" s="11">
         <f t="shared" si="5"/>
         <v>1650.104</v>
       </c>
@@ -3138,32 +3308,35 @@
         <f t="shared" si="1"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H60" s="40">
+      <c r="H60" s="12">
         <f t="shared" si="4"/>
         <v>1652.7923587563978</v>
       </c>
       <c r="I60" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J60" s="34">
+      <c r="J60" s="43">
         <f>((J59 * COUNT(C51:C60))-J59+C60)/COUNT(C51:C60)</f>
         <v>1662.0851752289673</v>
       </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K60" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="33">
         <v>41515</v>
       </c>
       <c r="B61" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C61" s="45">
+      <c r="C61" s="35">
         <v>1638.17</v>
       </c>
       <c r="D61" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E61" s="43">
+      <c r="E61" s="11">
         <f t="shared" si="5"/>
         <v>1647.789</v>
       </c>
@@ -3174,32 +3347,35 @@
         <f t="shared" si="1"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H61" s="40">
+      <c r="H61" s="12">
         <f t="shared" si="4"/>
         <v>1650.1337480734164</v>
       </c>
       <c r="I61" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J61" s="34">
+      <c r="J61" s="43">
         <f>((J60 * COUNT(C52:C61))-J60+C61)/COUNT(C52:C61)</f>
         <v>1659.6936577060703</v>
       </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K61" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="33">
         <v>41516</v>
       </c>
       <c r="B62" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C62" s="45">
+      <c r="C62" s="35">
         <v>1632.97</v>
       </c>
       <c r="D62" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E62" s="43">
+      <c r="E62" s="11">
         <f t="shared" si="5"/>
         <v>1645.5029999999999</v>
       </c>
@@ -3210,32 +3386,35 @@
         <f t="shared" si="1"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H62" s="40">
+      <c r="H62" s="12">
         <f t="shared" ref="H62:H93" si="6">G62*(C62-H61)+H61</f>
         <v>1647.0130666055225</v>
       </c>
       <c r="I62" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J62" s="34">
+      <c r="J62" s="43">
         <f>((J61 * COUNT(C53:C62))-J61+C62)/COUNT(C53:C62)</f>
         <v>1657.0212919354635</v>
       </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K62" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="33">
         <v>41520</v>
       </c>
       <c r="B63" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C63" s="45">
+      <c r="C63" s="35">
         <v>1639.77</v>
       </c>
       <c r="D63" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E63" s="43">
+      <c r="E63" s="11">
         <f t="shared" si="5"/>
         <v>1644.8739999999998</v>
       </c>
@@ -3246,32 +3425,35 @@
         <f t="shared" si="1"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H63" s="40">
+      <c r="H63" s="12">
         <f t="shared" si="6"/>
         <v>1645.6961454045183</v>
       </c>
       <c r="I63" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J63" s="34">
+      <c r="J63" s="43">
         <f>((J62 * COUNT(C54:C63))-J62+C63)/COUNT(C54:C63)</f>
         <v>1655.2961627419172</v>
       </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K63" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="33">
         <v>41521</v>
       </c>
       <c r="B64" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C64" s="45">
+      <c r="C64" s="35">
         <v>1653.08</v>
       </c>
       <c r="D64" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E64" s="43">
+      <c r="E64" s="11">
         <f t="shared" si="5"/>
         <v>1644.9470000000001</v>
       </c>
@@ -3282,32 +3464,35 @@
         <f t="shared" si="1"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H64" s="40">
+      <c r="H64" s="12">
         <f t="shared" si="6"/>
         <v>1647.0386644218786</v>
       </c>
       <c r="I64" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J64" s="34">
+      <c r="J64" s="43">
         <f>((J63 * COUNT(C55:C64))-J63+C64)/COUNT(C55:C64)</f>
         <v>1655.0745464677252</v>
       </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K64" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="33">
         <v>41522</v>
       </c>
       <c r="B65" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C65" s="45">
+      <c r="C65" s="35">
         <v>1655.08</v>
       </c>
       <c r="D65" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E65" s="43">
+      <c r="E65" s="11">
         <f t="shared" si="5"/>
         <v>1646.175</v>
       </c>
@@ -3318,32 +3503,35 @@
         <f t="shared" si="1"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H65" s="40">
+      <c r="H65" s="12">
         <f t="shared" si="6"/>
         <v>1648.5007254360826</v>
       </c>
       <c r="I65" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J65" s="34">
+      <c r="J65" s="43">
         <f>((J64 * COUNT(C56:C65))-J64+C65)/COUNT(C56:C65)</f>
         <v>1655.0750918209528</v>
       </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K65" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="33">
         <v>41523</v>
       </c>
       <c r="B66" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C66" s="45">
+      <c r="C66" s="35">
         <v>1655.17</v>
       </c>
       <c r="D66" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E66" s="43">
+      <c r="E66" s="11">
         <f t="shared" si="5"/>
         <v>1645.9959999999999</v>
       </c>
@@ -3354,32 +3542,35 @@
         <f t="shared" si="1"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H66" s="40">
+      <c r="H66" s="12">
         <f t="shared" si="6"/>
         <v>1649.7133208113403</v>
       </c>
       <c r="I66" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J66" s="34">
+      <c r="J66" s="43">
         <f>((J65 * COUNT(C57:C66))-J65+C66)/COUNT(C57:C66)</f>
         <v>1655.0845826388577</v>
       </c>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K66" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="33">
         <v>41526</v>
       </c>
       <c r="B67" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C67" s="45">
+      <c r="C67" s="35">
         <v>1671.71</v>
       </c>
       <c r="D67" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E67" s="43">
+      <c r="E67" s="11">
         <f t="shared" si="5"/>
         <v>1646.8170000000002</v>
       </c>
@@ -3390,32 +3581,35 @@
         <f t="shared" si="1"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H67" s="40">
+      <c r="H67" s="12">
         <f t="shared" si="6"/>
         <v>1653.7127170274603</v>
       </c>
       <c r="I67" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J67" s="34">
+      <c r="J67" s="43">
         <f>((J66 * COUNT(C58:C67))-J66+C67)/COUNT(C58:C67)</f>
         <v>1656.7471243749719</v>
       </c>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K67" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="33">
         <v>41527</v>
       </c>
       <c r="B68" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C68" s="45">
+      <c r="C68" s="35">
         <v>1683.99</v>
       </c>
       <c r="D68" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E68" s="43">
+      <c r="E68" s="11">
         <f t="shared" si="5"/>
         <v>1649.538</v>
       </c>
@@ -3426,32 +3620,35 @@
         <f t="shared" si="1"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H68" s="40">
+      <c r="H68" s="12">
         <f t="shared" si="6"/>
         <v>1659.217677567922</v>
       </c>
       <c r="I68" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J68" s="34">
+      <c r="J68" s="43">
         <f>((J67 * COUNT(C59:C68))-J67+C68)/COUNT(C59:C68)</f>
         <v>1659.4714119374748</v>
       </c>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K68" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="33">
         <v>41528</v>
       </c>
       <c r="B69" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C69" s="45">
+      <c r="C69" s="35">
         <v>1689.13</v>
       </c>
       <c r="D69" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E69" s="43">
+      <c r="E69" s="11">
         <f t="shared" si="5"/>
         <v>1655.4029999999998</v>
       </c>
@@ -3462,32 +3659,35 @@
         <f t="shared" si="1"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H69" s="40">
+      <c r="H69" s="12">
         <f t="shared" si="6"/>
         <v>1664.6562816464816</v>
       </c>
       <c r="I69" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J69" s="34">
+      <c r="J69" s="43">
         <f>((J68 * COUNT(C60:C69))-J68+C69)/COUNT(C60:C69)</f>
         <v>1662.4372707437274</v>
       </c>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K69" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="33">
         <v>41529</v>
       </c>
       <c r="B70" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C70" s="45">
+      <c r="C70" s="35">
         <v>1683.42</v>
       </c>
       <c r="D70" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E70" s="43">
+      <c r="E70" s="11">
         <f t="shared" si="5"/>
         <v>1660.2489999999998</v>
       </c>
@@ -3498,32 +3698,35 @@
         <f t="shared" si="1"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H70" s="40">
+      <c r="H70" s="12">
         <f t="shared" si="6"/>
         <v>1668.0678668016667</v>
       </c>
       <c r="I70" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J70" s="34">
+      <c r="J70" s="43">
         <f>((J69 * COUNT(C61:C70))-J69+C70)/COUNT(C61:C70)</f>
         <v>1664.5355436693546</v>
       </c>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K70" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="33">
         <v>41530</v>
       </c>
       <c r="B71" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C71" s="45">
+      <c r="C71" s="35">
         <v>1687.99</v>
       </c>
       <c r="D71" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E71" s="43">
+      <c r="E71" s="11">
         <f t="shared" si="5"/>
         <v>1665.2309999999998</v>
       </c>
@@ -3534,32 +3737,35 @@
         <f t="shared" si="1"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H71" s="40">
+      <c r="H71" s="12">
         <f t="shared" si="6"/>
         <v>1671.6900728377273</v>
       </c>
       <c r="I71" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J71" s="34">
+      <c r="J71" s="43">
         <f>((J70 * COUNT(C62:C71))-J70+C71)/COUNT(C62:C71)</f>
         <v>1666.880989302419</v>
       </c>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K71" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="33">
         <v>41533</v>
       </c>
       <c r="B72" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C72" s="45">
+      <c r="C72" s="35">
         <v>1697.6</v>
       </c>
       <c r="D72" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E72" s="43">
+      <c r="E72" s="11">
         <f t="shared" si="5"/>
         <v>1671.694</v>
       </c>
@@ -3570,32 +3776,35 @@
         <f t="shared" si="1"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H72" s="40">
+      <c r="H72" s="12">
         <f t="shared" si="6"/>
         <v>1676.4009686854131</v>
       </c>
       <c r="I72" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J72" s="34">
+      <c r="J72" s="43">
         <f>((J71 * COUNT(C63:C72))-J71+C72)/COUNT(C63:C72)</f>
         <v>1669.9528903721771</v>
       </c>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K72" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="33">
         <v>41534</v>
       </c>
       <c r="B73" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C73" s="45">
+      <c r="C73" s="35">
         <v>1704.76</v>
       </c>
       <c r="D73" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E73" s="43">
+      <c r="E73" s="11">
         <f t="shared" si="5"/>
         <v>1678.193</v>
       </c>
@@ -3606,32 +3815,35 @@
         <f t="shared" si="1"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H73" s="40">
+      <c r="H73" s="12">
         <f t="shared" si="6"/>
         <v>1681.5571561971562</v>
       </c>
       <c r="I73" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J73" s="34">
+      <c r="J73" s="43">
         <f>((J72 * COUNT(C64:C73))-J72+C73)/COUNT(C64:C73)</f>
         <v>1673.4336013349591</v>
       </c>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K73" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="33">
         <v>41535</v>
       </c>
       <c r="B74" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C74" s="45">
+      <c r="C74" s="35">
         <v>1725.52</v>
       </c>
       <c r="D74" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E74" s="43">
+      <c r="E74" s="11">
         <f t="shared" si="5"/>
         <v>1685.4369999999999</v>
       </c>
@@ -3642,32 +3854,35 @@
         <f t="shared" si="1"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H74" s="40">
+      <c r="H74" s="12">
         <f t="shared" si="6"/>
         <v>1689.5504005249461</v>
       </c>
       <c r="I74" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J74" s="34">
+      <c r="J74" s="43">
         <f>((J73 * COUNT(C65:C74))-J73+C74)/COUNT(C65:C74)</f>
         <v>1678.6422412014631</v>
       </c>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K74" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="33">
         <v>41536</v>
       </c>
       <c r="B75" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C75" s="45">
+      <c r="C75" s="35">
         <v>1722.34</v>
       </c>
       <c r="D75" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E75" s="43">
+      <c r="E75" s="11">
         <f t="shared" si="5"/>
         <v>1692.163</v>
       </c>
@@ -3678,32 +3893,35 @@
         <f t="shared" si="1"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H75" s="40">
+      <c r="H75" s="12">
         <f t="shared" si="6"/>
         <v>1695.5121458840467</v>
       </c>
       <c r="I75" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J75" s="34">
+      <c r="J75" s="43">
         <f>((J74 * COUNT(C66:C75))-J74+C75)/COUNT(C66:C75)</f>
         <v>1683.0120170813166</v>
       </c>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K75" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="33">
         <v>41537</v>
       </c>
       <c r="B76" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C76" s="45">
+      <c r="C76" s="35">
         <v>1709.91</v>
       </c>
       <c r="D76" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E76" s="43">
+      <c r="E76" s="11">
         <f t="shared" si="5"/>
         <v>1697.6370000000002</v>
       </c>
@@ -3714,32 +3932,35 @@
         <f t="shared" ref="G76:G112" si="7">2/(10+1)</f>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H76" s="40">
+      <c r="H76" s="12">
         <f t="shared" si="6"/>
         <v>1698.1299375414928</v>
       </c>
       <c r="I76" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J76" s="34">
+      <c r="J76" s="43">
         <f>((J75 * COUNT(C67:C76))-J75+C76)/COUNT(C67:C76)</f>
         <v>1685.7018153731849</v>
       </c>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K76" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="33">
         <v>41540</v>
       </c>
       <c r="B77" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C77" s="45">
+      <c r="C77" s="35">
         <v>1701.84</v>
       </c>
       <c r="D77" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E77" s="43">
+      <c r="E77" s="11">
         <f t="shared" ref="E77:E112" si="8">AVERAGE(C68:C77)</f>
         <v>1700.65</v>
       </c>
@@ -3750,32 +3971,35 @@
         <f t="shared" si="7"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H77" s="40">
+      <c r="H77" s="12">
         <f t="shared" si="6"/>
         <v>1698.8044943521304</v>
       </c>
       <c r="I77" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J77" s="34">
+      <c r="J77" s="43">
         <f>((J76 * COUNT(C68:C77))-J76+C77)/COUNT(C68:C77)</f>
         <v>1687.3156338358665</v>
       </c>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K77" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="33">
         <v>41541</v>
       </c>
       <c r="B78" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C78" s="45">
+      <c r="C78" s="35">
         <v>1697.42</v>
       </c>
       <c r="D78" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E78" s="43">
+      <c r="E78" s="11">
         <f t="shared" si="8"/>
         <v>1701.9929999999999</v>
       </c>
@@ -3786,32 +4010,35 @@
         <f t="shared" si="7"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H78" s="40">
+      <c r="H78" s="12">
         <f t="shared" si="6"/>
         <v>1698.5527681062886</v>
       </c>
       <c r="I78" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J78" s="34">
+      <c r="J78" s="43">
         <f>((J77 * COUNT(C69:C78))-J77+C78)/COUNT(C69:C78)</f>
         <v>1688.32607045228</v>
       </c>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K78" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="33">
         <v>41542</v>
       </c>
       <c r="B79" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C79" s="45">
+      <c r="C79" s="35">
         <v>1692.77</v>
       </c>
       <c r="D79" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E79" s="43">
+      <c r="E79" s="11">
         <f t="shared" si="8"/>
         <v>1702.357</v>
       </c>
@@ -3822,32 +4049,35 @@
         <f t="shared" si="7"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H79" s="40">
+      <c r="H79" s="12">
         <f t="shared" si="6"/>
         <v>1697.5013557233269</v>
       </c>
       <c r="I79" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J79" s="34">
+      <c r="J79" s="43">
         <f>((J78 * COUNT(C70:C79))-J78+C79)/COUNT(C70:C79)</f>
         <v>1688.7704634070519</v>
       </c>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K79" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="33">
         <v>41543</v>
       </c>
       <c r="B80" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C80" s="45">
+      <c r="C80" s="35">
         <v>1698.67</v>
       </c>
       <c r="D80" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E80" s="43">
+      <c r="E80" s="11">
         <f t="shared" si="8"/>
         <v>1703.8820000000001</v>
       </c>
@@ -3858,32 +4088,35 @@
         <f t="shared" si="7"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H80" s="40">
+      <c r="H80" s="12">
         <f t="shared" si="6"/>
         <v>1697.7138365009039</v>
       </c>
       <c r="I80" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J80" s="34">
+      <c r="J80" s="43">
         <f>((J79 * COUNT(C71:C80))-J79+C80)/COUNT(C71:C80)</f>
         <v>1689.7604170663467</v>
       </c>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K80" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="33">
         <v>41544</v>
       </c>
       <c r="B81" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C81" s="45">
+      <c r="C81" s="35">
         <v>1691.75</v>
       </c>
       <c r="D81" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E81" s="43">
+      <c r="E81" s="11">
         <f t="shared" si="8"/>
         <v>1704.2580000000003</v>
       </c>
@@ -3894,32 +4127,35 @@
         <f t="shared" si="7"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H81" s="40">
+      <c r="H81" s="12">
         <f t="shared" si="6"/>
         <v>1696.6295025916486</v>
       </c>
       <c r="I81" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J81" s="34">
+      <c r="J81" s="43">
         <f>((J80 * COUNT(C72:C81))-J80+C81)/COUNT(C72:C81)</f>
         <v>1689.9593753597121</v>
       </c>
-    </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K81" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="33">
         <v>41547</v>
       </c>
       <c r="B82" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C82" s="45">
+      <c r="C82" s="35">
         <v>1681.55</v>
       </c>
       <c r="D82" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E82" s="43">
+      <c r="E82" s="11">
         <f t="shared" si="8"/>
         <v>1702.6529999999998</v>
       </c>
@@ -3930,32 +4166,35 @@
         <f t="shared" si="7"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H82" s="40">
+      <c r="H82" s="12">
         <f t="shared" si="6"/>
         <v>1693.8877748477125</v>
       </c>
       <c r="I82" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J82" s="34">
+      <c r="J82" s="43">
         <f>((J81 * COUNT(C73:C82))-J81+C82)/COUNT(C73:C82)</f>
         <v>1689.1184378237408</v>
       </c>
-    </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K82" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="33">
         <v>41548</v>
       </c>
       <c r="B83" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C83" s="45">
+      <c r="C83" s="35">
         <v>1695</v>
       </c>
       <c r="D83" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E83" s="43">
+      <c r="E83" s="11">
         <f t="shared" si="8"/>
         <v>1701.6769999999997</v>
       </c>
@@ -3966,32 +4205,35 @@
         <f t="shared" si="7"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H83" s="40">
+      <c r="H83" s="12">
         <f t="shared" si="6"/>
         <v>1694.089997602674</v>
       </c>
       <c r="I83" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J83" s="34">
+      <c r="J83" s="43">
         <f>((J82 * COUNT(C74:C83))-J82+C83)/COUNT(C74:C83)</f>
         <v>1689.7065940413668</v>
       </c>
-    </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K83" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="33">
         <v>41549</v>
       </c>
       <c r="B84" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C84" s="45">
+      <c r="C84" s="35">
         <v>1693.87</v>
       </c>
       <c r="D84" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E84" s="43">
+      <c r="E84" s="11">
         <f t="shared" si="8"/>
         <v>1698.5119999999999</v>
       </c>
@@ -4002,32 +4244,35 @@
         <f t="shared" si="7"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H84" s="40">
+      <c r="H84" s="12">
         <f t="shared" si="6"/>
         <v>1694.0499980385514</v>
       </c>
       <c r="I84" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J84" s="34">
+      <c r="J84" s="43">
         <f>((J83 * COUNT(C75:C84))-J83+C84)/COUNT(C75:C84)</f>
         <v>1690.1229346372299</v>
       </c>
-    </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K84" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="33">
         <v>41550</v>
       </c>
       <c r="B85" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C85" s="45">
+      <c r="C85" s="35">
         <v>1678.66</v>
       </c>
       <c r="D85" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E85" s="43">
+      <c r="E85" s="11">
         <f t="shared" si="8"/>
         <v>1694.1439999999998</v>
       </c>
@@ -4038,32 +4283,35 @@
         <f t="shared" si="7"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H85" s="40">
+      <c r="H85" s="12">
         <f t="shared" si="6"/>
         <v>1691.2518165769966</v>
       </c>
       <c r="I85" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J85" s="34">
+      <c r="J85" s="43">
         <f>((J84 * COUNT(C76:C85))-J84+C85)/COUNT(C76:C85)</f>
         <v>1688.9766411735072</v>
       </c>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K85" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="33">
         <v>41551</v>
       </c>
       <c r="B86" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C86" s="45">
+      <c r="C86" s="35">
         <v>1690.5</v>
       </c>
       <c r="D86" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E86" s="43">
+      <c r="E86" s="11">
         <f t="shared" si="8"/>
         <v>1692.203</v>
       </c>
@@ -4074,32 +4322,35 @@
         <f t="shared" si="7"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H86" s="40">
+      <c r="H86" s="12">
         <f t="shared" si="6"/>
         <v>1691.1151226539064</v>
       </c>
       <c r="I86" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J86" s="34">
+      <c r="J86" s="43">
         <f>((J85 * COUNT(C77:C86))-J85+C86)/COUNT(C77:C86)</f>
         <v>1689.1289770561566</v>
       </c>
-    </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K86" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" s="33">
         <v>41554</v>
       </c>
       <c r="B87" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C87" s="45">
+      <c r="C87" s="35">
         <v>1676.12</v>
       </c>
       <c r="D87" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E87" s="43">
+      <c r="E87" s="11">
         <f t="shared" si="8"/>
         <v>1689.6309999999999</v>
       </c>
@@ -4110,32 +4361,35 @@
         <f t="shared" si="7"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H87" s="40">
+      <c r="H87" s="12">
         <f t="shared" si="6"/>
         <v>1688.3887367168325</v>
       </c>
       <c r="I87" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J87" s="34">
+      <c r="J87" s="43">
         <f>((J86 * COUNT(C78:C87))-J86+C87)/COUNT(C78:C87)</f>
         <v>1687.8280793505407</v>
       </c>
-    </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K87" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="33">
         <v>41555</v>
       </c>
       <c r="B88" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C88" s="45">
+      <c r="C88" s="35">
         <v>1655.45</v>
       </c>
       <c r="D88" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E88" s="43">
+      <c r="E88" s="11">
         <f t="shared" si="8"/>
         <v>1685.434</v>
       </c>
@@ -4146,32 +4400,35 @@
         <f t="shared" si="7"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H88" s="40">
+      <c r="H88" s="12">
         <f t="shared" si="6"/>
         <v>1682.3998754955901</v>
       </c>
       <c r="I88" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J88" s="34">
+      <c r="J88" s="43">
         <f>((J87 * COUNT(C79:C88))-J87+C88)/COUNT(C79:C88)</f>
         <v>1684.5902714154868</v>
       </c>
-    </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K88" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="33">
         <v>41556</v>
       </c>
       <c r="B89" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C89" s="45">
+      <c r="C89" s="35">
         <v>1656.4</v>
       </c>
       <c r="D89" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E89" s="43">
+      <c r="E89" s="11">
         <f t="shared" si="8"/>
         <v>1681.797</v>
       </c>
@@ -4182,32 +4439,35 @@
         <f t="shared" si="7"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H89" s="40">
+      <c r="H89" s="12">
         <f t="shared" si="6"/>
         <v>1677.6726254054829</v>
       </c>
       <c r="I89" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J89" s="34">
+      <c r="J89" s="43">
         <f>((J88 * COUNT(C80:C89))-J88+C89)/COUNT(C80:C89)</f>
         <v>1681.7712442739382</v>
       </c>
-    </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K89" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="33">
         <v>41557</v>
       </c>
       <c r="B90" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C90" s="45">
+      <c r="C90" s="35">
         <v>1692.56</v>
       </c>
       <c r="D90" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E90" s="43">
+      <c r="E90" s="11">
         <f t="shared" si="8"/>
         <v>1681.1860000000001</v>
       </c>
@@ -4218,32 +4478,35 @@
         <f t="shared" si="7"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H90" s="40">
+      <c r="H90" s="12">
         <f t="shared" si="6"/>
         <v>1680.3794207863041</v>
       </c>
       <c r="I90" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J90" s="34">
+      <c r="J90" s="43">
         <f>((J89 * COUNT(C81:C90))-J89+C90)/COUNT(C81:C90)</f>
         <v>1682.8501198465444</v>
       </c>
-    </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K90" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="33">
         <v>41558</v>
       </c>
       <c r="B91" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C91" s="45">
+      <c r="C91" s="35">
         <v>1703.2</v>
       </c>
       <c r="D91" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E91" s="43">
+      <c r="E91" s="11">
         <f t="shared" si="8"/>
         <v>1682.3310000000001</v>
       </c>
@@ -4254,32 +4517,35 @@
         <f t="shared" si="7"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H91" s="40">
+      <c r="H91" s="12">
         <f t="shared" si="6"/>
         <v>1684.528617006976</v>
       </c>
       <c r="I91" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J91" s="34">
+      <c r="J91" s="43">
         <f>((J90 * COUNT(C82:C91))-J90+C91)/COUNT(C82:C91)</f>
         <v>1684.88510786189</v>
       </c>
-    </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K91" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="33">
         <v>41561</v>
       </c>
       <c r="B92" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C92" s="45">
+      <c r="C92" s="35">
         <v>1710.14</v>
       </c>
       <c r="D92" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E92" s="43">
+      <c r="E92" s="11">
         <f t="shared" si="8"/>
         <v>1685.19</v>
       </c>
@@ -4290,32 +4556,35 @@
         <f t="shared" si="7"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H92" s="40">
+      <c r="H92" s="12">
         <f t="shared" si="6"/>
         <v>1689.1852320966168</v>
       </c>
       <c r="I92" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J92" s="34">
+      <c r="J92" s="43">
         <f>((J91 * COUNT(C83:C92))-J91+C92)/COUNT(C83:C92)</f>
         <v>1687.4105970757009</v>
       </c>
-    </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K92" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="33">
         <v>41562</v>
       </c>
       <c r="B93" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C93" s="45">
+      <c r="C93" s="35">
         <v>1698.06</v>
       </c>
       <c r="D93" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E93" s="43">
+      <c r="E93" s="11">
         <f t="shared" si="8"/>
         <v>1685.4959999999999</v>
       </c>
@@ -4326,32 +4595,35 @@
         <f t="shared" si="7"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H93" s="40">
+      <c r="H93" s="12">
         <f t="shared" si="6"/>
         <v>1690.7988262608683</v>
       </c>
       <c r="I93" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J93" s="34">
+      <c r="J93" s="43">
         <f>((J92 * COUNT(C84:C93))-J92+C93)/COUNT(C84:C93)</f>
         <v>1688.475537368131</v>
       </c>
-    </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K93" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="33">
         <v>41563</v>
       </c>
       <c r="B94" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C94" s="45">
+      <c r="C94" s="35">
         <v>1721.54</v>
       </c>
       <c r="D94" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E94" s="43">
+      <c r="E94" s="11">
         <f t="shared" si="8"/>
         <v>1688.2629999999997</v>
       </c>
@@ -4362,32 +4634,35 @@
         <f t="shared" si="7"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H94" s="40">
+      <c r="H94" s="12">
         <f t="shared" ref="H94:H112" si="9">G94*(C94-H93)+H93</f>
         <v>1696.388130577074</v>
       </c>
       <c r="I94" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J94" s="34">
+      <c r="J94" s="43">
         <f>((J93 * COUNT(C85:C94))-J93+C94)/COUNT(C85:C94)</f>
         <v>1691.7819836313179</v>
       </c>
-    </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K94" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" s="33">
         <v>41564</v>
       </c>
       <c r="B95" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C95" s="45">
+      <c r="C95" s="35">
         <v>1733.15</v>
       </c>
       <c r="D95" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E95" s="43">
+      <c r="E95" s="11">
         <f t="shared" si="8"/>
         <v>1693.712</v>
       </c>
@@ -4398,32 +4673,35 @@
         <f t="shared" si="7"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H95" s="40">
+      <c r="H95" s="12">
         <f t="shared" si="9"/>
         <v>1703.0721068357877</v>
       </c>
       <c r="I95" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J95" s="34">
+      <c r="J95" s="43">
         <f>((J94 * COUNT(C86:C95))-J94+C95)/COUNT(C86:C95)</f>
         <v>1695.9187852681862</v>
       </c>
-    </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K95" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" s="33">
         <v>41565</v>
       </c>
       <c r="B96" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C96" s="45">
+      <c r="C96" s="35">
         <v>1744.5</v>
       </c>
       <c r="D96" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E96" s="43">
+      <c r="E96" s="11">
         <f t="shared" si="8"/>
         <v>1699.1119999999996</v>
       </c>
@@ -4434,32 +4712,35 @@
         <f t="shared" si="7"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H96" s="40">
+      <c r="H96" s="12">
         <f t="shared" si="9"/>
         <v>1710.6044510474626</v>
       </c>
       <c r="I96" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J96" s="34">
+      <c r="J96" s="43">
         <f>((J95 * COUNT(C87:C96))-J95+C96)/COUNT(C87:C96)</f>
         <v>1700.7769067413676</v>
       </c>
-    </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K96" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" s="33">
         <v>41568</v>
       </c>
       <c r="B97" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C97" s="45">
+      <c r="C97" s="35">
         <v>1744.66</v>
       </c>
       <c r="D97" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E97" s="43">
+      <c r="E97" s="11">
         <f t="shared" si="8"/>
         <v>1705.9659999999999</v>
       </c>
@@ -4470,32 +4751,35 @@
         <f t="shared" si="7"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H97" s="40">
+      <c r="H97" s="12">
         <f t="shared" si="9"/>
         <v>1716.7963690388331</v>
       </c>
       <c r="I97" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J97" s="34">
+      <c r="J97" s="43">
         <f>((J96 * COUNT(C88:C97))-J96+C97)/COUNT(C88:C97)</f>
         <v>1705.1652160672306</v>
       </c>
-    </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K97" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" s="33">
         <v>41569</v>
       </c>
       <c r="B98" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C98" s="45">
+      <c r="C98" s="35">
         <v>1754.67</v>
       </c>
       <c r="D98" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E98" s="43">
+      <c r="E98" s="11">
         <f t="shared" si="8"/>
         <v>1715.8880000000001</v>
       </c>
@@ -4506,32 +4790,35 @@
         <f t="shared" si="7"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H98" s="40">
+      <c r="H98" s="12">
         <f t="shared" si="9"/>
         <v>1723.6824837590452</v>
       </c>
       <c r="I98" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J98" s="34">
+      <c r="J98" s="43">
         <f>((J97 * COUNT(C89:C98))-J97+C98)/COUNT(C89:C98)</f>
         <v>1710.1156944605077</v>
       </c>
-    </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K98" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" s="33">
         <v>41570</v>
       </c>
       <c r="B99" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C99" s="45">
+      <c r="C99" s="35">
         <v>1746.38</v>
       </c>
       <c r="D99" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E99" s="43">
+      <c r="E99" s="11">
         <f t="shared" si="8"/>
         <v>1724.886</v>
       </c>
@@ -4542,32 +4829,35 @@
         <f t="shared" si="7"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H99" s="40">
+      <c r="H99" s="12">
         <f t="shared" si="9"/>
         <v>1727.8093048937642</v>
       </c>
       <c r="I99" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J99" s="34">
+      <c r="J99" s="43">
         <f>((J98 * COUNT(C90:C99))-J98+C99)/COUNT(C90:C99)</f>
         <v>1713.7421250144569</v>
       </c>
-    </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K99" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" s="33">
         <v>41571</v>
       </c>
       <c r="B100" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C100" s="45">
+      <c r="C100" s="35">
         <v>1752.07</v>
       </c>
       <c r="D100" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E100" s="43">
+      <c r="E100" s="11">
         <f t="shared" si="8"/>
         <v>1730.837</v>
       </c>
@@ -4578,32 +4868,35 @@
         <f t="shared" si="7"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H100" s="40">
+      <c r="H100" s="12">
         <f t="shared" si="9"/>
         <v>1732.2203403676253</v>
       </c>
       <c r="I100" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J100" s="34">
+      <c r="J100" s="43">
         <f>((J99 * COUNT(C91:C100))-J99+C100)/COUNT(C91:C100)</f>
         <v>1717.5749125130114</v>
       </c>
-    </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K100" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" s="33">
         <v>41572</v>
       </c>
       <c r="B101" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C101" s="45">
+      <c r="C101" s="35">
         <v>1759.77</v>
       </c>
       <c r="D101" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E101" s="43">
+      <c r="E101" s="11">
         <f t="shared" si="8"/>
         <v>1736.4939999999999</v>
       </c>
@@ -4614,32 +4907,35 @@
         <f t="shared" si="7"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H101" s="40">
+      <c r="H101" s="12">
         <f t="shared" si="9"/>
         <v>1737.2293693916934</v>
       </c>
       <c r="I101" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J101" s="34">
+      <c r="J101" s="43">
         <f>((J100 * COUNT(C92:C101))-J100+C101)/COUNT(C92:C101)</f>
         <v>1721.7944212617101</v>
       </c>
-    </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K101" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" s="33">
         <v>41575</v>
       </c>
       <c r="B102" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C102" s="45">
+      <c r="C102" s="35">
         <v>1762.11</v>
       </c>
       <c r="D102" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E102" s="43">
+      <c r="E102" s="11">
         <f t="shared" si="8"/>
         <v>1741.691</v>
       </c>
@@ -4650,32 +4946,35 @@
         <f t="shared" si="7"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H102" s="40">
+      <c r="H102" s="12">
         <f t="shared" si="9"/>
         <v>1741.7531204113855</v>
       </c>
       <c r="I102" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J102" s="34">
+      <c r="J102" s="43">
         <f>((J101 * COUNT(C93:C102))-J101+C102)/COUNT(C93:C102)</f>
         <v>1725.825979135539</v>
       </c>
-    </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K102" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" s="33">
         <v>41576</v>
       </c>
       <c r="B103" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C103" s="45">
+      <c r="C103" s="35">
         <v>1771.95</v>
       </c>
       <c r="D103" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E103" s="43">
+      <c r="E103" s="11">
         <f t="shared" si="8"/>
         <v>1749.0800000000004</v>
       </c>
@@ -4686,32 +4985,35 @@
         <f t="shared" si="7"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H103" s="40">
+      <c r="H103" s="12">
         <f t="shared" si="9"/>
         <v>1747.24346215477</v>
       </c>
       <c r="I103" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J103" s="34">
+      <c r="J103" s="43">
         <f>((J102 * COUNT(C94:C103))-J102+C103)/COUNT(C94:C103)</f>
         <v>1730.4383812219851</v>
       </c>
-    </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K103" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" s="33">
         <v>41577</v>
       </c>
       <c r="B104" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C104" s="45">
+      <c r="C104" s="35">
         <v>1763.31</v>
       </c>
       <c r="D104" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E104" s="43">
+      <c r="E104" s="11">
         <f t="shared" si="8"/>
         <v>1753.2570000000003</v>
       </c>
@@ -4722,32 +5024,35 @@
         <f t="shared" si="7"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H104" s="40">
+      <c r="H104" s="12">
         <f t="shared" si="9"/>
         <v>1750.1646508539027</v>
       </c>
       <c r="I104" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J104" s="34">
+      <c r="J104" s="43">
         <f>((J103 * COUNT(C95:C104))-J103+C104)/COUNT(C95:C104)</f>
         <v>1733.7255430997866</v>
       </c>
-    </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K104" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" s="33">
         <v>41578</v>
       </c>
       <c r="B105" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C105" s="45">
+      <c r="C105" s="35">
         <v>1756.54</v>
       </c>
       <c r="D105" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E105" s="43">
+      <c r="E105" s="11">
         <f t="shared" si="8"/>
         <v>1755.5960000000002</v>
       </c>
@@ -4758,32 +5063,35 @@
         <f t="shared" si="7"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H105" s="40">
+      <c r="H105" s="12">
         <f t="shared" si="9"/>
         <v>1751.3238052441022</v>
       </c>
       <c r="I105" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J105" s="34">
+      <c r="J105" s="43">
         <f>((J104 * COUNT(C96:C105))-J104+C105)/COUNT(C96:C105)</f>
         <v>1736.006988789808</v>
       </c>
-    </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K105" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" s="33">
         <v>41579</v>
       </c>
       <c r="B106" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C106" s="45">
+      <c r="C106" s="35">
         <v>1761.64</v>
       </c>
       <c r="D106" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E106" s="43">
+      <c r="E106" s="11">
         <f t="shared" si="8"/>
         <v>1757.31</v>
       </c>
@@ -4794,32 +5102,35 @@
         <f t="shared" si="7"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H106" s="40">
+      <c r="H106" s="12">
         <f t="shared" si="9"/>
         <v>1753.1994770179019</v>
       </c>
       <c r="I106" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J106" s="34">
+      <c r="J106" s="43">
         <f>((J105 * COUNT(C97:C106))-J105+C106)/COUNT(C97:C106)</f>
         <v>1738.5702899108273</v>
       </c>
-    </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K106" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" s="33">
         <v>41582</v>
       </c>
       <c r="B107" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C107" s="45">
+      <c r="C107" s="35">
         <v>1767.93</v>
       </c>
       <c r="D107" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E107" s="43">
+      <c r="E107" s="11">
         <f t="shared" si="8"/>
         <v>1759.6369999999999</v>
       </c>
@@ -4830,32 +5141,35 @@
         <f t="shared" si="7"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H107" s="40">
+      <c r="H107" s="12">
         <f t="shared" si="9"/>
         <v>1755.8777539237381</v>
       </c>
       <c r="I107" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J107" s="34">
+      <c r="J107" s="43">
         <f>((J106 * COUNT(C98:C107))-J106+C107)/COUNT(C98:C107)</f>
         <v>1741.5062609197444</v>
       </c>
-    </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K107" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" s="33">
         <v>41583</v>
       </c>
       <c r="B108" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C108" s="45">
+      <c r="C108" s="35">
         <v>1762.97</v>
       </c>
       <c r="D108" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E108" s="43">
+      <c r="E108" s="11">
         <f t="shared" si="8"/>
         <v>1760.4669999999999</v>
       </c>
@@ -4866,32 +5180,35 @@
         <f t="shared" si="7"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H108" s="40">
+      <c r="H108" s="12">
         <f t="shared" si="9"/>
         <v>1757.1672532103312</v>
       </c>
       <c r="I108" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J108" s="34">
+      <c r="J108" s="43">
         <f>((J107 * COUNT(C99:C108))-J107+C108)/COUNT(C99:C108)</f>
         <v>1743.65263482777</v>
       </c>
-    </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K108" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" s="33">
         <v>41584</v>
       </c>
       <c r="B109" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C109" s="45">
+      <c r="C109" s="35">
         <v>1770.49</v>
       </c>
       <c r="D109" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E109" s="43">
+      <c r="E109" s="11">
         <f t="shared" si="8"/>
         <v>1762.8779999999999</v>
       </c>
@@ -4902,32 +5219,35 @@
         <f t="shared" si="7"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H109" s="40">
+      <c r="H109" s="12">
         <f t="shared" si="9"/>
         <v>1759.5895708084529</v>
       </c>
       <c r="I109" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J109" s="34">
+      <c r="J109" s="43">
         <f>((J108 * COUNT(C100:C109))-J108+C109)/COUNT(C100:C109)</f>
         <v>1746.3363713449933</v>
       </c>
-    </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K109" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" s="33">
         <v>41585</v>
       </c>
       <c r="B110" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C110" s="45">
+      <c r="C110" s="35">
         <v>1747.15</v>
       </c>
       <c r="D110" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E110" s="43">
+      <c r="E110" s="11">
         <f t="shared" si="8"/>
         <v>1762.386</v>
       </c>
@@ -4938,32 +5258,35 @@
         <f t="shared" si="7"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H110" s="40">
+      <c r="H110" s="12">
         <f t="shared" si="9"/>
         <v>1757.3278306614616</v>
       </c>
       <c r="I110" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J110" s="34">
+      <c r="J110" s="43">
         <f>((J109 * COUNT(C101:C110))-J109+C110)/COUNT(C101:C110)</f>
         <v>1746.417734210494</v>
       </c>
-    </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K110" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" s="33">
         <v>41586</v>
       </c>
       <c r="B111" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C111" s="45">
+      <c r="C111" s="35">
         <v>1770.61</v>
       </c>
       <c r="D111" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E111" s="43">
+      <c r="E111" s="11">
         <f t="shared" si="8"/>
         <v>1763.4699999999998</v>
       </c>
@@ -4974,32 +5297,35 @@
         <f t="shared" si="7"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H111" s="40">
+      <c r="H111" s="12">
         <f t="shared" si="9"/>
         <v>1759.7427705411958</v>
       </c>
       <c r="I111" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J111" s="34">
+      <c r="J111" s="43">
         <f>((J110 * COUNT(C102:C111))-J110+C111)/COUNT(C102:C111)</f>
         <v>1748.8369607894444</v>
       </c>
-    </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K111" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" s="33">
         <v>41589</v>
       </c>
       <c r="B112" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C112" s="45">
+      <c r="C112" s="35">
         <v>1771.89</v>
       </c>
       <c r="D112" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E112" s="43">
+      <c r="E112" s="11">
         <f t="shared" si="8"/>
         <v>1764.4479999999999</v>
       </c>
@@ -5010,24 +5336,27 @@
         <f t="shared" si="7"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H112" s="40">
+      <c r="H112" s="12">
         <f t="shared" si="9"/>
         <v>1761.951357715524</v>
       </c>
       <c r="I112" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J112" s="34">
+      <c r="J112" s="43">
         <f>((J111 * COUNT(C103:C112))-J111+C112)/COUNT(C103:C112)</f>
         <v>1751.1422647105003</v>
       </c>
+      <c r="K112" s="9" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="113" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C113" s="45">
+      <c r="C113" s="35">
         <f>COUNT(C3:C112)</f>
         <v>110</v>
       </c>
-      <c r="E113" s="43">
+      <c r="E113" s="11">
         <f>COUNTIF(E3:E112, "&gt;0")</f>
         <v>100</v>
       </c>
@@ -5035,7 +5364,7 @@
         <f>COUNTIF(G3:G112, "&gt;0")</f>
         <v>109</v>
       </c>
-      <c r="H113" s="40">
+      <c r="H113" s="12">
         <f>COUNTIF(H3:H112, "&gt;0")</f>
         <v>100</v>
       </c>

</xml_diff>